<commit_message>
update ds rule import data
</commit_message>
<xml_diff>
--- a/public/assets/format/format_import_ds.xlsx
+++ b/public/assets/format/format_import_ds.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yi-order-system\public\assets\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>customer_code</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>2022-07-06</t>
+  </si>
+  <si>
+    <t>percentage</t>
   </si>
 </sst>
 </file>
@@ -363,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -375,9 +378,10 @@
     <col min="2" max="2" width="32.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -390,8 +394,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -400,6 +407,9 @@
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="E2">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>